<commit_message>
refactor(invoicing): SAV-1028: Added support for ImagingArea product category
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/refdata-valid-invoice-product-and-sources.xlsx
+++ b/packages/central-server/__tests__/importers/refdata-valid-invoice-product-and-sources.xlsx
@@ -5,15 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice Product" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Drug" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Lab Test Type" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Lab Test Category" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Lab Test Panel" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Procedure Type" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Imaging Type" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="X Ray Imaging Area" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Drug" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Lab Test Type" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Lab Test Category" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Lab Test Panel" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Procedure Type" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="108">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -131,7 +133,7 @@
     <t xml:space="preserve">procedure-34831</t>
   </si>
   <si>
-    <t xml:space="preserve">Procedure</t>
+    <t xml:space="preserve">ProcedureType</t>
   </si>
   <si>
     <r>
@@ -166,6 +168,42 @@
   </si>
   <si>
     <t xml:space="preserve">Drug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvoiceProduct-imagingType-xRay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImagingType-xRay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Ray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImagingType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvoiceProduct-imagingArea-xRay-foot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImagingArea-xRay-foot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Ray Foot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xRayImagingArea-foot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImagingArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xRay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xray-foot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foot</t>
   </si>
   <si>
     <t xml:space="preserve">drug-asparaginase10000</t>
@@ -533,11 +571,11 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24"/>
@@ -659,6 +697,52 @@
         <v>1</v>
       </c>
       <c r="G5" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1658,154 +1742,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1823,6 +1788,217 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1842,37 +2018,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,7 +2062,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>135</v>
@@ -1901,27 +2077,27 @@
         <v>146</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>3.5</v>
@@ -1936,27 +2112,27 @@
         <v>5.3</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>95</v>
@@ -1971,27 +2147,27 @@
         <v>106</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>17</v>
@@ -2006,27 +2182,27 @@
         <v>29</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>4.2</v>
@@ -2035,13 +2211,13 @@
         <v>6.1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2060,7 +2236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2089,13 +2265,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -2115,7 +2291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2142,13 +2318,13 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,13 +2341,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2200,7 +2376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2229,13 +2405,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>34830</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2246,95 +2422,95 @@
         <v>34831</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>34832</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>35081</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>35082</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>35091</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>35092</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>35102</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>35103</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>23900</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>